<commit_message>
10.03. Spawning Rocket Trails
</commit_message>
<xml_diff>
--- a/data/Weapon.xlsx
+++ b/data/Weapon.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Rifle</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Rocket Launcher</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -90,7 +96,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -98,12 +104,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -384,120 +412,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
10.05. Hit Scan Weapons
</commit_message>
<xml_diff>
--- a/data/Weapon.xlsx
+++ b/data/Weapon.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Rifle</t>
   </si>
   <si>
-    <t>Aim Spread Modifier</t>
-  </si>
-  <si>
     <t>Default Spread in Degrees</t>
   </si>
   <si>
@@ -72,6 +69,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Pistol</t>
+  </si>
+  <si>
+    <t>Aim Speed Modifier</t>
   </si>
 </sst>
 </file>
@@ -412,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,19 +426,23 @@
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.109375" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>0.5</v>
@@ -443,10 +450,13 @@
       <c r="C2" s="3">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -454,10 +464,13 @@
       <c r="C3" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -465,10 +478,13 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>45</v>
@@ -476,10 +492,13 @@
       <c r="C5" s="3">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>20</v>
@@ -487,10 +506,13 @@
       <c r="C6" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>0.5</v>
@@ -498,10 +520,13 @@
       <c r="C7" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>0.8</v>
@@ -509,10 +534,13 @@
       <c r="C8" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
@@ -520,21 +548,27 @@
       <c r="C9" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>0.15</v>
@@ -542,10 +576,13 @@
       <c r="C11" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>30</v>
@@ -553,16 +590,22 @@
       <c r="C12" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="3">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>